<commit_message>
+ BPMNComponents now save their creation time + BpmnComponents can be compared based on creation time +added Codewriter class which writes a python file (transformation part) + added codewriter to Engine, Token, startevent +CS & TS have new need func get_code -> returns string with python code +added get_code to all cs & ts +token now calls codewriter when needed + token id reworked so it can be used as a variable in generated code +added SelectStrategy + Strategyfactory can now create Select & Filter +Function parser new dt plain_text *func_parser new func for function with variable parameters , puts them ->into a list and can also check if all have the same needed dt +examplefiles and logs updated
</commit_message>
<xml_diff>
--- a/Notebooks/inktest.xlsx
+++ b/Notebooks/inktest.xlsx
@@ -512,36 +512,36 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>09.Jan</t>
+          <t>05.Jan</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>P2</t>
+          <t>P1</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>K1</t>
+          <t>K2</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>11.Jan</t>
+          <t>07.Jan</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -551,47 +551,47 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>P2</t>
+          <t>P1</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>K1</t>
+          <t>K2</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>05.Jan</t>
+          <t>09.Jan</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>P1</t>
+          <t>P2</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>K2</t>
+          <t>K1</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>07.Jan</t>
+          <t>11.Jan</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -601,12 +601,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>P1</t>
+          <t>P2</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>K2</t>
+          <t>K1</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed issue with concat
</commit_message>
<xml_diff>
--- a/Notebooks/inktest.xlsx
+++ b/Notebooks/inktest.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,6 +459,11 @@
           <t>Kostenstelle</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Demo</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -484,6 +489,11 @@
           <t>unknown</t>
         </is>
       </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>lÃ¤uft gut</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -509,6 +519,11 @@
           <t>unknown</t>
         </is>
       </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>lÃ¤uft gut</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -534,6 +549,11 @@
           <t>K2</t>
         </is>
       </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>lÃ¤uft gut</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -559,6 +579,11 @@
           <t>K2</t>
         </is>
       </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>lÃ¤uft gut</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -584,6 +609,11 @@
           <t>K1</t>
         </is>
       </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>lÃ¤uft gut</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -607,6 +637,11 @@
       <c r="E7" t="inlineStr">
         <is>
           <t>K1</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>lÃ¤uft gut</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
prio and query now seperated from each other
</commit_message>
<xml_diff>
--- a/Notebooks/inktest.xlsx
+++ b/Notebooks/inktest.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,11 +459,6 @@
           <t>Kostenstelle</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Demo</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -489,11 +484,6 @@
           <t>unknown</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>lÃ¤uft gut</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -519,11 +509,6 @@
           <t>unknown</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>lÃ¤uft gut</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -549,11 +534,6 @@
           <t>K2</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>lÃ¤uft gut</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -579,11 +559,6 @@
           <t>K2</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>lÃ¤uft gut</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -609,11 +584,6 @@
           <t>K1</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>lÃ¤uft gut</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -637,11 +607,6 @@
       <c r="E7" t="inlineStr">
         <is>
           <t>K1</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>lÃ¤uft gut</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
refactoring bpmn components fixed flow prioritiese
</commit_message>
<xml_diff>
--- a/Notebooks/inktest.xlsx
+++ b/Notebooks/inktest.xlsx
@@ -462,36 +462,36 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>06.Jan</t>
+          <t>05.Jan</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>A</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>P3</t>
+          <t>P1</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>K2</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>10.Jan</t>
+          <t>07.Jan</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -501,47 +501,47 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>P3</t>
+          <t>P1</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>K2</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>05.Jan</t>
+          <t>09.Jan</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>B</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>P1</t>
+          <t>P2</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>K2</t>
+          <t>K1</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>07.Jan</t>
+          <t>11.Jan</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -551,22 +551,22 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>P1</t>
+          <t>P2</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>K2</t>
+          <t>K1</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>09.Jan</t>
+          <t>06.Jan</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -576,22 +576,22 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>P2</t>
+          <t>P3</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>K1</t>
+          <t>unknown</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>11.Jan</t>
+          <t>10.Jan</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -601,12 +601,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>P2</t>
+          <t>P3</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>K1</t>
+          <t>unknown</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
task function redesign completed prep for expr function prep for combinestrats
</commit_message>
<xml_diff>
--- a/Notebooks/inktest.xlsx
+++ b/Notebooks/inktest.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>CC_UNKNOWN</t>
         </is>
       </c>
     </row>
@@ -606,7 +606,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>unknown</t>
+          <t>CC_UNKNOWN</t>
         </is>
       </c>
     </row>

</xml_diff>